<commit_message>
1. Export chart data 2. Adjust excel report
</commit_message>
<xml_diff>
--- a/report_template/daily_report.xlsx
+++ b/report_template/daily_report.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t>監測日報表</t>
   </si>
@@ -142,16 +142,15 @@
     <t>定保</t>
   </si>
   <si>
-    <t>無效數據</t>
+    <t>異常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>校正失敗</t>
+    <t>自動檢核</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>不可抗力</t>
-  </si>
-  <si>
-    <t>遺失資料</t>
+    <t>人工註記</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -194,18 +193,12 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -233,13 +226,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="8" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,6 +291,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -305,18 +301,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
@@ -336,6 +320,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,8 +442,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="263414368"/>
-        <c:axId val="263409272"/>
+        <c:axId val="209287232"/>
+        <c:axId val="209288016"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -498,11 +491,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="263412016"/>
-        <c:axId val="263408096"/>
+        <c:axId val="207143712"/>
+        <c:axId val="207149200"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="263414368"/>
+        <c:axId val="209287232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +523,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263409272"/>
+        <c:crossAx val="209288016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -538,7 +531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="263409272"/>
+        <c:axId val="209288016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -568,12 +561,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263414368"/>
+        <c:crossAx val="209287232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="263408096"/>
+        <c:axId val="207149200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -604,13 +597,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263412016"/>
+        <c:crossAx val="207143712"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="263412016"/>
+        <c:axId val="207143712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,7 +612,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263408096"/>
+        <c:crossAx val="207149200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -857,8 +850,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="263411624"/>
-        <c:axId val="263408488"/>
+        <c:axId val="206753760"/>
+        <c:axId val="206756112"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -906,11 +899,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="263412408"/>
-        <c:axId val="263408880"/>
+        <c:axId val="210210432"/>
+        <c:axId val="428845280"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="263411624"/>
+        <c:axId val="206753760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263408488"/>
+        <c:crossAx val="206756112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -946,7 +939,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="263408488"/>
+        <c:axId val="206756112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -976,12 +969,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263411624"/>
+        <c:crossAx val="206753760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="263408880"/>
+        <c:axId val="428845280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -1012,13 +1005,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263412408"/>
+        <c:crossAx val="210210432"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="263412408"/>
+        <c:axId val="210210432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1027,7 +1020,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263408880"/>
+        <c:crossAx val="428845280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1096,6 +1089,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1264,8 +1258,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="263122520"/>
-        <c:axId val="263122912"/>
+        <c:axId val="209292328"/>
+        <c:axId val="423349976"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1313,11 +1307,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="265438152"/>
-        <c:axId val="263120560"/>
+        <c:axId val="423351936"/>
+        <c:axId val="423354288"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="263122520"/>
+        <c:axId val="209292328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,12 +1333,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263122912"/>
+        <c:crossAx val="423349976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1352,7 +1347,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="263122912"/>
+        <c:axId val="423349976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,18 +1370,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263122520"/>
+        <c:crossAx val="209292328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="263120560"/>
+        <c:axId val="423354288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -1410,19 +1406,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265438152"/>
+        <c:crossAx val="423351936"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265438152"/>
+        <c:axId val="423351936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1431,13 +1428,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263120560"/>
+        <c:crossAx val="423354288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1499,6 +1497,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1667,8 +1666,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="265438544"/>
-        <c:axId val="265439328"/>
+        <c:axId val="423353112"/>
+        <c:axId val="423355072"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1716,11 +1715,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="265439720"/>
-        <c:axId val="265443248"/>
+        <c:axId val="423353896"/>
+        <c:axId val="423353504"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="265438544"/>
+        <c:axId val="423353112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1742,12 +1741,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265439328"/>
+        <c:crossAx val="423355072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1755,7 +1755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="265439328"/>
+        <c:axId val="423355072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1778,18 +1778,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265438544"/>
+        <c:crossAx val="423353112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265443248"/>
+        <c:axId val="423353504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -1813,19 +1814,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265439720"/>
+        <c:crossAx val="423353896"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265439720"/>
+        <c:axId val="423353896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,13 +1836,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265443248"/>
+        <c:crossAx val="423353504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1902,6 +1905,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2070,8 +2074,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="265437760"/>
-        <c:axId val="265440896"/>
+        <c:axId val="423356640"/>
+        <c:axId val="423357032"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2119,11 +2123,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="265440112"/>
-        <c:axId val="265438936"/>
+        <c:axId val="423350760"/>
+        <c:axId val="423357424"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="265437760"/>
+        <c:axId val="423356640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2145,12 +2149,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265440896"/>
+        <c:crossAx val="423357032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2158,7 +2163,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="265440896"/>
+        <c:axId val="423357032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,18 +2186,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265437760"/>
+        <c:crossAx val="423356640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265438936"/>
+        <c:axId val="423357424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -2216,19 +2222,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265440112"/>
+        <c:crossAx val="423350760"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265440112"/>
+        <c:axId val="423350760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2237,13 +2244,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265438936"/>
+        <c:crossAx val="423357424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2317,6 +2325,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2485,8 +2494,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="263410056"/>
-        <c:axId val="263412800"/>
+        <c:axId val="423351152"/>
+        <c:axId val="423351544"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2534,11 +2543,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="265211728"/>
-        <c:axId val="263413192"/>
+        <c:axId val="208549368"/>
+        <c:axId val="423355856"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="263410056"/>
+        <c:axId val="423351152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2560,12 +2569,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263412800"/>
+        <c:crossAx val="423351544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2573,7 +2583,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="263412800"/>
+        <c:axId val="423351544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2596,18 +2606,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263410056"/>
+        <c:crossAx val="423351152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="263413192"/>
+        <c:axId val="423355856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -2631,19 +2642,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265211728"/>
+        <c:crossAx val="208549368"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265211728"/>
+        <c:axId val="208549368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2652,13 +2664,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="263413192"/>
+        <c:crossAx val="423355856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2720,6 +2733,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2888,8 +2902,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="265212512"/>
-        <c:axId val="265214472"/>
+        <c:axId val="429773584"/>
+        <c:axId val="502544288"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2937,11 +2951,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="265215256"/>
-        <c:axId val="265211336"/>
+        <c:axId val="502543112"/>
+        <c:axId val="502541936"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="265212512"/>
+        <c:axId val="429773584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2963,12 +2977,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265214472"/>
+        <c:crossAx val="502544288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2976,7 +2991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="265214472"/>
+        <c:axId val="502544288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2999,18 +3014,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265212512"/>
+        <c:crossAx val="429773584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265211336"/>
+        <c:axId val="502541936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -3034,19 +3050,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265215256"/>
+        <c:crossAx val="502543112"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265215256"/>
+        <c:axId val="502543112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3055,13 +3072,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265211336"/>
+        <c:crossAx val="502541936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3120,6 +3138,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3288,8 +3307,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="265217216"/>
-        <c:axId val="265213688"/>
+        <c:axId val="502539192"/>
+        <c:axId val="502544680"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3337,11 +3356,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="265210552"/>
-        <c:axId val="265214864"/>
+        <c:axId val="502545072"/>
+        <c:axId val="502540760"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="265217216"/>
+        <c:axId val="502539192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3363,12 +3382,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265213688"/>
+        <c:crossAx val="502544680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3376,7 +3396,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="265213688"/>
+        <c:axId val="502544680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3399,18 +3419,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265217216"/>
+        <c:crossAx val="502539192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265214864"/>
+        <c:axId val="502540760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -3434,19 +3455,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265210552"/>
+        <c:crossAx val="502545072"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265210552"/>
+        <c:axId val="502545072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3455,13 +3477,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265214864"/>
+        <c:crossAx val="502540760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4010,8 +4033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -4022,26 +4045,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -4053,26 +4076,26 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -4084,20 +4107,20 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
       <c r="H3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="18" t="s">
         <v>32</v>
       </c>
       <c r="K3" s="10" t="s">
@@ -4106,18 +4129,16 @@
       <c r="L3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="14" t="s">
+      <c r="N3" s="9" t="s">
         <v>36</v>
       </c>
+      <c r="O3" s="19"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
@@ -4211,23 +4232,23 @@
       <c r="A5" s="5">
         <v>0</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1">
@@ -4256,23 +4277,23 @@
       <c r="A6" s="5">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1">
@@ -4301,23 +4322,23 @@
       <c r="A7" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1">
@@ -4346,23 +4367,23 @@
       <c r="A8" s="5">
         <v>0.125</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1">
@@ -4391,23 +4412,23 @@
       <c r="A9" s="5">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1">
@@ -4436,23 +4457,23 @@
       <c r="A10" s="5">
         <v>0.20833333333333334</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1">
@@ -4481,23 +4502,23 @@
       <c r="A11" s="5">
         <v>0.25</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1">
@@ -4526,23 +4547,23 @@
       <c r="A12" s="5">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1">
@@ -4571,23 +4592,23 @@
       <c r="A13" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1">
@@ -4616,23 +4637,23 @@
       <c r="A14" s="5">
         <v>0.375</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1">
@@ -4661,23 +4682,23 @@
       <c r="A15" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1">
@@ -4706,23 +4727,23 @@
       <c r="A16" s="5">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1">
@@ -4751,23 +4772,23 @@
       <c r="A17" s="5">
         <v>0.5</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1">
@@ -4796,23 +4817,23 @@
       <c r="A18" s="5">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1">
@@ -4841,23 +4862,23 @@
       <c r="A19" s="5">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1">
@@ -4886,23 +4907,23 @@
       <c r="A20" s="5">
         <v>0.625</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1">
@@ -4931,23 +4952,23 @@
       <c r="A21" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1">
@@ -4976,23 +4997,23 @@
       <c r="A22" s="5">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1">
@@ -5021,23 +5042,23 @@
       <c r="A23" s="5">
         <v>0.75</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1">
@@ -5066,23 +5087,23 @@
       <c r="A24" s="5">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1">
@@ -5111,23 +5132,23 @@
       <c r="A25" s="5">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1">
@@ -5156,23 +5177,23 @@
       <c r="A26" s="5">
         <v>0.875</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1">
@@ -5201,23 +5222,23 @@
       <c r="A27" s="5">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1">
@@ -5246,23 +5267,23 @@
       <c r="A28" s="5">
         <v>0.95833333333333337</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1">
@@ -5291,23 +5312,23 @@
       <c r="A29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
@@ -5322,23 +5343,23 @@
       <c r="A30" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
@@ -5353,23 +5374,23 @@
       <c r="A31" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
@@ -5384,23 +5405,23 @@
       <c r="A32" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
@@ -5619,26 +5640,26 @@
       <c r="AA35" s="1"/>
     </row>
     <row r="36" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="17"/>
-      <c r="P36" s="17"/>
-      <c r="Q36" s="17"/>
-      <c r="R36" s="17"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
@@ -5650,24 +5671,24 @@
       <c r="AA36" s="1"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="17"/>
-      <c r="R37" s="17"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
@@ -5679,24 +5700,24 @@
       <c r="AA37" s="1"/>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
-      <c r="Q38" s="17"/>
-      <c r="R38" s="17"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
@@ -5708,24 +5729,24 @@
       <c r="AA38" s="1"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17"/>
-      <c r="Q39" s="17"/>
-      <c r="R39" s="17"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
@@ -5737,24 +5758,24 @@
       <c r="AA39" s="1"/>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="17"/>
-      <c r="P40" s="17"/>
-      <c r="Q40" s="17"/>
-      <c r="R40" s="17"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>

</xml_diff>

<commit_message>
1. Re-org auditor rules 2. Remove auto audit from excel
</commit_message>
<xml_diff>
--- a/report_template/daily_report.xlsx
+++ b/report_template/daily_report.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
   <si>
     <t>監測日報表</t>
   </si>
@@ -146,10 +146,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>自動檢核</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>人工註記</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -208,7 +204,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,12 +238,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,7 +291,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -342,9 +332,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4150,7 +4137,7 @@
   <dimension ref="A1:AD40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -4162,29 +4149,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
@@ -4196,29 +4183,29 @@
       <c r="AD1" s="1"/>
     </row>
     <row r="2" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -4230,8 +4217,8 @@
       <c r="AD2" s="1"/>
     </row>
     <row r="3" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
@@ -4250,14 +4237,12 @@
       <c r="H3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>36</v>
-      </c>
+      <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -4266,7 +4251,6 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
     </row>
     <row r="4" spans="1:30" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -4300,10 +4284,10 @@
         <v>11</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>12</v>
@@ -4312,7 +4296,7 @@
         <v>13</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>14</v>
@@ -5873,29 +5857,29 @@
       <c r="AD35" s="1"/>
     </row>
     <row r="36" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="17"/>
-      <c r="P36" s="17"/>
-      <c r="Q36" s="17"/>
-      <c r="R36" s="17"/>
-      <c r="S36" s="17"/>
-      <c r="T36" s="17"/>
-      <c r="U36" s="17"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
@@ -5907,27 +5891,27 @@
       <c r="AD36" s="1"/>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="17"/>
-      <c r="R37" s="17"/>
-      <c r="S37" s="17"/>
-      <c r="T37" s="17"/>
-      <c r="U37" s="17"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+      <c r="T37" s="16"/>
+      <c r="U37" s="16"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
@@ -5939,27 +5923,27 @@
       <c r="AD37" s="1"/>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
-      <c r="Q38" s="17"/>
-      <c r="R38" s="17"/>
-      <c r="S38" s="17"/>
-      <c r="T38" s="17"/>
-      <c r="U38" s="17"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
@@ -5971,27 +5955,27 @@
       <c r="AD38" s="1"/>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17"/>
-      <c r="Q39" s="17"/>
-      <c r="R39" s="17"/>
-      <c r="S39" s="17"/>
-      <c r="T39" s="17"/>
-      <c r="U39" s="17"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
@@ -6003,27 +5987,27 @@
       <c r="AD39" s="1"/>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="17"/>
-      <c r="P40" s="17"/>
-      <c r="Q40" s="17"/>
-      <c r="R40" s="17"/>
-      <c r="S40" s="17"/>
-      <c r="T40" s="17"/>
-      <c r="U40" s="17"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="16"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
@@ -6041,7 +6025,7 @@
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="T2:U2"/>
-    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="S3:T3"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
1. 簡訊通知 2. NOY, NOY-NO, NH3 日月年報
</commit_message>
<xml_diff>
--- a/report_template/daily_report.xlsx
+++ b/report_template/daily_report.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
   <si>
     <t>監測日報表</t>
   </si>
@@ -161,6 +161,16 @@
   </si>
   <si>
     <t>氨
+ppb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOY
+ppb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NH3
 ppb</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -422,7 +432,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$P$4</c:f>
+              <c:f>監測日報表!$S$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -450,7 +460,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測日報表!$P$5:$P$28</c:f>
+              <c:f>監測日報表!$S$5:$S$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="24"/>
@@ -485,7 +495,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$Q$4</c:f>
+              <c:f>監測日報表!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -506,7 +516,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測日報表!$Q$5:$Q$28</c:f>
+              <c:f>監測日報表!$T$5:$T$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="24"/>
@@ -774,7 +784,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$X$4</c:f>
+              <c:f>監測日報表!$AA$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -796,7 +806,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測日報表!$X$5:$X$28</c:f>
+              <c:f>監測日報表!$AA$5:$AA$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -903,7 +913,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$Q$4</c:f>
+              <c:f>監測日報表!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -924,7 +934,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測日報表!$Q$5:$Q$28</c:f>
+              <c:f>監測日報表!$T$5:$T$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="24"/>
@@ -1192,7 +1202,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$Y$4</c:f>
+              <c:f>監測日報表!$AB$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1214,7 +1224,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測日報表!$Y$5:$Y$28</c:f>
+              <c:f>監測日報表!$AB$5:$AB$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1321,7 +1331,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$Q$4</c:f>
+              <c:f>監測日報表!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1342,7 +1352,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測日報表!$Q$5:$Q$28</c:f>
+              <c:f>監測日報表!$T$5:$T$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="24"/>
@@ -1610,7 +1620,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$Z$4</c:f>
+              <c:f>監測日報表!$AC$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1632,7 +1642,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測日報表!$Z$5:$Z$28</c:f>
+              <c:f>監測日報表!$AC$5:$AC$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1739,7 +1749,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$Q$4</c:f>
+              <c:f>監測日報表!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1760,7 +1770,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測日報表!$Q$5:$Q$28</c:f>
+              <c:f>監測日報表!$T$5:$T$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="24"/>
@@ -2028,7 +2038,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$AA$4</c:f>
+              <c:f>監測日報表!$AD$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2050,7 +2060,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測日報表!$AA$5:$AA$28</c:f>
+              <c:f>監測日報表!$AD$5:$AD$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -2157,7 +2167,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$Q$4</c:f>
+              <c:f>監測日報表!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2178,7 +2188,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測日報表!$Q$5:$Q$28</c:f>
+              <c:f>監測日報表!$T$5:$T$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="24"/>
@@ -2411,7 +2421,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$N$4</c:f>
+              <c:f>監測日報表!$Q$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2439,7 +2449,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測日報表!$N$5:$N$28</c:f>
+              <c:f>監測日報表!$Q$5:$Q$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="24"/>
@@ -2458,7 +2468,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$AB$4</c:f>
+              <c:f>監測日報表!$AE$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2480,7 +2490,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測日報表!$AB$5:$AB$28</c:f>
+              <c:f>監測日報表!$AE$5:$AE$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -2587,7 +2597,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$Q$4</c:f>
+              <c:f>監測日報表!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2608,7 +2618,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測日報表!$Q$5:$Q$28</c:f>
+              <c:f>監測日報表!$T$5:$T$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="24"/>
@@ -2876,7 +2886,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$AC$4</c:f>
+              <c:f>監測日報表!$AF$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2898,7 +2908,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測日報表!$AC$5:$AC$28</c:f>
+              <c:f>監測日報表!$AF$5:$AF$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -3005,7 +3015,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$Q$4</c:f>
+              <c:f>監測日報表!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3026,7 +3036,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測日報表!$Q$5:$Q$28</c:f>
+              <c:f>監測日報表!$T$5:$T$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="24"/>
@@ -3244,7 +3254,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$M$4</c:f>
+              <c:f>監測日報表!$P$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3272,7 +3282,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測日報表!$M$5:$M$28</c:f>
+              <c:f>監測日報表!$P$5:$P$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="24"/>
@@ -3291,7 +3301,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$AD$4</c:f>
+              <c:f>監測日報表!$AG$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3313,7 +3323,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測日報表!$AD$5:$AD$28</c:f>
+              <c:f>監測日報表!$AG$5:$AG$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -3420,7 +3430,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測日報表!$Q$4</c:f>
+              <c:f>監測日報表!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3441,7 +3451,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測日報表!$Q$5:$Q$28</c:f>
+              <c:f>監測日報表!$T$5:$T$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="24"/>
@@ -3642,8 +3652,8 @@
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -3702,8 +3712,8 @@
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>92</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -3762,8 +3772,8 @@
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>118</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -3822,8 +3832,8 @@
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>143</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -4134,21 +4144,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD40"/>
+  <dimension ref="A1:AG40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="11.125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.25" customWidth="1"/>
-    <col min="16" max="30" width="11.125" customWidth="1" collapsed="1"/>
+    <col min="1" max="11" width="11.125" customWidth="1" collapsed="1"/>
+    <col min="12" max="14" width="11.125" customWidth="1"/>
+    <col min="15" max="16" width="11.125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.25" customWidth="1"/>
+    <col min="19" max="33" width="11.125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -4172,17 +4184,20 @@
       <c r="S1" s="17"/>
       <c r="T1" s="17"/>
       <c r="U1" s="17"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
@@ -4204,19 +4219,22 @@
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
       <c r="S2" s="18"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="21"/>
       <c r="C3" s="3" t="s">
@@ -4237,22 +4255,22 @@
       <c r="H3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -4287,46 +4305,46 @@
         <v>38</v>
       </c>
       <c r="L4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="U4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
       <c r="AA4" s="1" t="s">
         <v>23</v>
       </c>
@@ -4339,8 +4357,17 @@
       <c r="AD4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="AE4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>0</v>
       </c>
@@ -4364,31 +4391,34 @@
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1">
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1">
         <v>20</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="AB5" s="1">
         <v>10</v>
       </c>
-      <c r="Z5" s="1">
+      <c r="AC5" s="1">
         <v>50</v>
       </c>
-      <c r="AA5" s="1">
+      <c r="AD5" s="1">
         <v>120</v>
       </c>
-      <c r="AB5" s="1">
+      <c r="AE5" s="1">
         <v>125</v>
       </c>
-      <c r="AC5" s="1">
+      <c r="AF5" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD5" s="1">
+      <c r="AG5" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -4412,31 +4442,34 @@
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1">
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1">
         <v>20</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="AB6" s="1">
         <v>10</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="AC6" s="1">
         <v>50</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AD6" s="1">
         <v>120</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AE6" s="1">
         <v>125</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AF6" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD6" s="1">
+      <c r="AG6" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -4460,31 +4493,34 @@
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1">
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1">
         <v>20</v>
       </c>
-      <c r="Y7" s="1">
+      <c r="AB7" s="1">
         <v>10</v>
       </c>
-      <c r="Z7" s="1">
+      <c r="AC7" s="1">
         <v>50</v>
       </c>
-      <c r="AA7" s="1">
+      <c r="AD7" s="1">
         <v>120</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AE7" s="1">
         <v>125</v>
       </c>
-      <c r="AC7" s="1">
+      <c r="AF7" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD7" s="1">
+      <c r="AG7" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>0.125</v>
       </c>
@@ -4508,31 +4544,34 @@
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1">
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1">
         <v>20</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="AB8" s="1">
         <v>10</v>
       </c>
-      <c r="Z8" s="1">
+      <c r="AC8" s="1">
         <v>50</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="AD8" s="1">
         <v>120</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AE8" s="1">
         <v>125</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AF8" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD8" s="1">
+      <c r="AG8" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>0.16666666666666666</v>
       </c>
@@ -4556,31 +4595,34 @@
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
       <c r="U9" s="8"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1">
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1">
         <v>20</v>
       </c>
-      <c r="Y9" s="1">
+      <c r="AB9" s="1">
         <v>10</v>
       </c>
-      <c r="Z9" s="1">
+      <c r="AC9" s="1">
         <v>50</v>
       </c>
-      <c r="AA9" s="1">
+      <c r="AD9" s="1">
         <v>120</v>
       </c>
-      <c r="AB9" s="1">
+      <c r="AE9" s="1">
         <v>125</v>
       </c>
-      <c r="AC9" s="1">
+      <c r="AF9" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD9" s="1">
+      <c r="AG9" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>0.20833333333333334</v>
       </c>
@@ -4604,31 +4646,34 @@
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1">
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1">
         <v>20</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="AB10" s="1">
         <v>10</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="AC10" s="1">
         <v>50</v>
       </c>
-      <c r="AA10" s="1">
+      <c r="AD10" s="1">
         <v>120</v>
       </c>
-      <c r="AB10" s="1">
+      <c r="AE10" s="1">
         <v>125</v>
       </c>
-      <c r="AC10" s="1">
+      <c r="AF10" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD10" s="1">
+      <c r="AG10" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>0.25</v>
       </c>
@@ -4652,31 +4697,34 @@
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1">
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1">
         <v>20</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="AB11" s="1">
         <v>10</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="AC11" s="1">
         <v>50</v>
       </c>
-      <c r="AA11" s="1">
+      <c r="AD11" s="1">
         <v>120</v>
       </c>
-      <c r="AB11" s="1">
+      <c r="AE11" s="1">
         <v>125</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AF11" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD11" s="1">
+      <c r="AG11" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>0.29166666666666669</v>
       </c>
@@ -4700,31 +4748,34 @@
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1">
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1">
         <v>20</v>
       </c>
-      <c r="Y12" s="1">
+      <c r="AB12" s="1">
         <v>10</v>
       </c>
-      <c r="Z12" s="1">
+      <c r="AC12" s="1">
         <v>50</v>
       </c>
-      <c r="AA12" s="1">
+      <c r="AD12" s="1">
         <v>120</v>
       </c>
-      <c r="AB12" s="1">
+      <c r="AE12" s="1">
         <v>125</v>
       </c>
-      <c r="AC12" s="1">
+      <c r="AF12" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD12" s="1">
+      <c r="AG12" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>0.33333333333333331</v>
       </c>
@@ -4748,31 +4799,34 @@
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1">
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1">
         <v>20</v>
       </c>
-      <c r="Y13" s="1">
+      <c r="AB13" s="1">
         <v>10</v>
       </c>
-      <c r="Z13" s="1">
+      <c r="AC13" s="1">
         <v>50</v>
       </c>
-      <c r="AA13" s="1">
+      <c r="AD13" s="1">
         <v>120</v>
       </c>
-      <c r="AB13" s="1">
+      <c r="AE13" s="1">
         <v>125</v>
       </c>
-      <c r="AC13" s="1">
+      <c r="AF13" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD13" s="1">
+      <c r="AG13" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>0.375</v>
       </c>
@@ -4796,31 +4850,34 @@
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
       <c r="U14" s="8"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1">
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1">
         <v>20</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="AB14" s="1">
         <v>10</v>
       </c>
-      <c r="Z14" s="1">
+      <c r="AC14" s="1">
         <v>50</v>
       </c>
-      <c r="AA14" s="1">
+      <c r="AD14" s="1">
         <v>120</v>
       </c>
-      <c r="AB14" s="1">
+      <c r="AE14" s="1">
         <v>125</v>
       </c>
-      <c r="AC14" s="1">
+      <c r="AF14" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD14" s="1">
+      <c r="AG14" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>0.41666666666666669</v>
       </c>
@@ -4844,31 +4901,34 @@
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1">
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1">
         <v>20</v>
       </c>
-      <c r="Y15" s="1">
+      <c r="AB15" s="1">
         <v>10</v>
       </c>
-      <c r="Z15" s="1">
+      <c r="AC15" s="1">
         <v>50</v>
       </c>
-      <c r="AA15" s="1">
+      <c r="AD15" s="1">
         <v>120</v>
       </c>
-      <c r="AB15" s="1">
+      <c r="AE15" s="1">
         <v>125</v>
       </c>
-      <c r="AC15" s="1">
+      <c r="AF15" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD15" s="1">
+      <c r="AG15" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>0.45833333333333331</v>
       </c>
@@ -4892,31 +4952,34 @@
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
       <c r="U16" s="8"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1">
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1">
         <v>20</v>
       </c>
-      <c r="Y16" s="1">
+      <c r="AB16" s="1">
         <v>10</v>
       </c>
-      <c r="Z16" s="1">
+      <c r="AC16" s="1">
         <v>50</v>
       </c>
-      <c r="AA16" s="1">
+      <c r="AD16" s="1">
         <v>120</v>
       </c>
-      <c r="AB16" s="1">
+      <c r="AE16" s="1">
         <v>125</v>
       </c>
-      <c r="AC16" s="1">
+      <c r="AF16" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD16" s="1">
+      <c r="AG16" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>0.5</v>
       </c>
@@ -4940,31 +5003,34 @@
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1">
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1">
         <v>20</v>
       </c>
-      <c r="Y17" s="1">
+      <c r="AB17" s="1">
         <v>10</v>
       </c>
-      <c r="Z17" s="1">
+      <c r="AC17" s="1">
         <v>50</v>
       </c>
-      <c r="AA17" s="1">
+      <c r="AD17" s="1">
         <v>120</v>
       </c>
-      <c r="AB17" s="1">
+      <c r="AE17" s="1">
         <v>125</v>
       </c>
-      <c r="AC17" s="1">
+      <c r="AF17" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD17" s="1">
+      <c r="AG17" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>0.54166666666666663</v>
       </c>
@@ -4988,31 +5054,34 @@
       <c r="S18" s="8"/>
       <c r="T18" s="8"/>
       <c r="U18" s="8"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1">
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1">
         <v>20</v>
       </c>
-      <c r="Y18" s="1">
+      <c r="AB18" s="1">
         <v>10</v>
       </c>
-      <c r="Z18" s="1">
+      <c r="AC18" s="1">
         <v>50</v>
       </c>
-      <c r="AA18" s="1">
+      <c r="AD18" s="1">
         <v>120</v>
       </c>
-      <c r="AB18" s="1">
+      <c r="AE18" s="1">
         <v>125</v>
       </c>
-      <c r="AC18" s="1">
+      <c r="AF18" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD18" s="1">
+      <c r="AG18" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>0.58333333333333337</v>
       </c>
@@ -5036,31 +5105,34 @@
       <c r="S19" s="8"/>
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1">
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1">
         <v>20</v>
       </c>
-      <c r="Y19" s="1">
+      <c r="AB19" s="1">
         <v>10</v>
       </c>
-      <c r="Z19" s="1">
+      <c r="AC19" s="1">
         <v>50</v>
       </c>
-      <c r="AA19" s="1">
+      <c r="AD19" s="1">
         <v>120</v>
       </c>
-      <c r="AB19" s="1">
+      <c r="AE19" s="1">
         <v>125</v>
       </c>
-      <c r="AC19" s="1">
+      <c r="AF19" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD19" s="1">
+      <c r="AG19" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>0.625</v>
       </c>
@@ -5084,31 +5156,34 @@
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
       <c r="U20" s="8"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1">
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1">
         <v>20</v>
       </c>
-      <c r="Y20" s="1">
+      <c r="AB20" s="1">
         <v>10</v>
       </c>
-      <c r="Z20" s="1">
+      <c r="AC20" s="1">
         <v>50</v>
       </c>
-      <c r="AA20" s="1">
+      <c r="AD20" s="1">
         <v>120</v>
       </c>
-      <c r="AB20" s="1">
+      <c r="AE20" s="1">
         <v>125</v>
       </c>
-      <c r="AC20" s="1">
+      <c r="AF20" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD20" s="1">
+      <c r="AG20" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>0.66666666666666663</v>
       </c>
@@ -5132,31 +5207,34 @@
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
       <c r="U21" s="8"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1">
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1">
         <v>20</v>
       </c>
-      <c r="Y21" s="1">
+      <c r="AB21" s="1">
         <v>10</v>
       </c>
-      <c r="Z21" s="1">
+      <c r="AC21" s="1">
         <v>50</v>
       </c>
-      <c r="AA21" s="1">
+      <c r="AD21" s="1">
         <v>120</v>
       </c>
-      <c r="AB21" s="1">
+      <c r="AE21" s="1">
         <v>125</v>
       </c>
-      <c r="AC21" s="1">
+      <c r="AF21" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD21" s="1">
+      <c r="AG21" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>0.70833333333333337</v>
       </c>
@@ -5180,31 +5258,34 @@
       <c r="S22" s="8"/>
       <c r="T22" s="8"/>
       <c r="U22" s="8"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1">
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1">
         <v>20</v>
       </c>
-      <c r="Y22" s="1">
+      <c r="AB22" s="1">
         <v>10</v>
       </c>
-      <c r="Z22" s="1">
+      <c r="AC22" s="1">
         <v>50</v>
       </c>
-      <c r="AA22" s="1">
+      <c r="AD22" s="1">
         <v>120</v>
       </c>
-      <c r="AB22" s="1">
+      <c r="AE22" s="1">
         <v>125</v>
       </c>
-      <c r="AC22" s="1">
+      <c r="AF22" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD22" s="1">
+      <c r="AG22" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>0.75</v>
       </c>
@@ -5228,31 +5309,34 @@
       <c r="S23" s="8"/>
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1">
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1">
         <v>20</v>
       </c>
-      <c r="Y23" s="1">
+      <c r="AB23" s="1">
         <v>10</v>
       </c>
-      <c r="Z23" s="1">
+      <c r="AC23" s="1">
         <v>50</v>
       </c>
-      <c r="AA23" s="1">
+      <c r="AD23" s="1">
         <v>120</v>
       </c>
-      <c r="AB23" s="1">
+      <c r="AE23" s="1">
         <v>125</v>
       </c>
-      <c r="AC23" s="1">
+      <c r="AF23" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD23" s="1">
+      <c r="AG23" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>0.79166666666666663</v>
       </c>
@@ -5276,31 +5360,34 @@
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1">
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1">
         <v>20</v>
       </c>
-      <c r="Y24" s="1">
+      <c r="AB24" s="1">
         <v>10</v>
       </c>
-      <c r="Z24" s="1">
+      <c r="AC24" s="1">
         <v>50</v>
       </c>
-      <c r="AA24" s="1">
+      <c r="AD24" s="1">
         <v>120</v>
       </c>
-      <c r="AB24" s="1">
+      <c r="AE24" s="1">
         <v>125</v>
       </c>
-      <c r="AC24" s="1">
+      <c r="AF24" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD24" s="1">
+      <c r="AG24" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>0.83333333333333337</v>
       </c>
@@ -5324,31 +5411,34 @@
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1">
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1">
         <v>20</v>
       </c>
-      <c r="Y25" s="1">
+      <c r="AB25" s="1">
         <v>10</v>
       </c>
-      <c r="Z25" s="1">
+      <c r="AC25" s="1">
         <v>50</v>
       </c>
-      <c r="AA25" s="1">
+      <c r="AD25" s="1">
         <v>120</v>
       </c>
-      <c r="AB25" s="1">
+      <c r="AE25" s="1">
         <v>125</v>
       </c>
-      <c r="AC25" s="1">
+      <c r="AF25" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD25" s="1">
+      <c r="AG25" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>0.875</v>
       </c>
@@ -5372,31 +5462,34 @@
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
       <c r="U26" s="8"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1">
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1">
         <v>20</v>
       </c>
-      <c r="Y26" s="1">
+      <c r="AB26" s="1">
         <v>10</v>
       </c>
-      <c r="Z26" s="1">
+      <c r="AC26" s="1">
         <v>50</v>
       </c>
-      <c r="AA26" s="1">
+      <c r="AD26" s="1">
         <v>120</v>
       </c>
-      <c r="AB26" s="1">
+      <c r="AE26" s="1">
         <v>125</v>
       </c>
-      <c r="AC26" s="1">
+      <c r="AF26" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD26" s="1">
+      <c r="AG26" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>0.91666666666666663</v>
       </c>
@@ -5420,31 +5513,34 @@
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
       <c r="U27" s="8"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1">
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1">
         <v>20</v>
       </c>
-      <c r="Y27" s="1">
+      <c r="AB27" s="1">
         <v>10</v>
       </c>
-      <c r="Z27" s="1">
+      <c r="AC27" s="1">
         <v>50</v>
       </c>
-      <c r="AA27" s="1">
+      <c r="AD27" s="1">
         <v>120</v>
       </c>
-      <c r="AB27" s="1">
+      <c r="AE27" s="1">
         <v>125</v>
       </c>
-      <c r="AC27" s="1">
+      <c r="AF27" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD27" s="1">
+      <c r="AG27" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>0.95833333333333337</v>
       </c>
@@ -5468,31 +5564,34 @@
       <c r="S28" s="8"/>
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1">
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="8"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1">
         <v>20</v>
       </c>
-      <c r="Y28" s="1">
+      <c r="AB28" s="1">
         <v>10</v>
       </c>
-      <c r="Z28" s="1">
+      <c r="AC28" s="1">
         <v>50</v>
       </c>
-      <c r="AA28" s="1">
+      <c r="AD28" s="1">
         <v>120</v>
       </c>
-      <c r="AB28" s="1">
+      <c r="AE28" s="1">
         <v>125</v>
       </c>
-      <c r="AC28" s="1">
+      <c r="AF28" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD28" s="1">
+      <c r="AG28" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>20</v>
       </c>
@@ -5516,17 +5615,20 @@
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
       <c r="U29" s="8"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+      <c r="AG29" s="1"/>
     </row>
-    <row r="30" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>21</v>
       </c>
@@ -5550,17 +5652,20 @@
       <c r="S30" s="8"/>
       <c r="T30" s="8"/>
       <c r="U30" s="8"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+      <c r="AF30" s="1"/>
+      <c r="AG30" s="1"/>
     </row>
-    <row r="31" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>22</v>
       </c>
@@ -5584,17 +5689,20 @@
       <c r="S31" s="8"/>
       <c r="T31" s="8"/>
       <c r="U31" s="8"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+      <c r="AF31" s="1"/>
+      <c r="AG31" s="1"/>
     </row>
-    <row r="32" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>24</v>
       </c>
@@ -5618,17 +5726,20 @@
       <c r="S32" s="8"/>
       <c r="T32" s="8"/>
       <c r="U32" s="8"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="X32" s="1"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="1"/>
+      <c r="AG32" s="1"/>
     </row>
-    <row r="33" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>25</v>
       </c>
@@ -5665,22 +5776,22 @@
       <c r="L33" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M33" s="7">
+      <c r="M33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P33" s="7">
         <v>250</v>
       </c>
-      <c r="N33" s="7">
+      <c r="Q33" s="7">
         <v>125</v>
       </c>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q33" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R33" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="R33" s="7"/>
       <c r="S33" s="7" t="s">
         <v>26</v>
       </c>
@@ -5690,17 +5801,26 @@
       <c r="U33" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
+      <c r="V33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X33" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+      <c r="AF33" s="1"/>
+      <c r="AG33" s="1"/>
     </row>
-    <row r="34" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>27</v>
       </c>
@@ -5741,24 +5861,24 @@
       <c r="L34" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M34" s="7">
-        <f>COUNTIF(M5:M28,"&gt;"&amp;M33)</f>
+      <c r="M34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P34" s="7">
+        <f>COUNTIF(P5:P28,"&gt;"&amp;P33)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="7">
-        <f>COUNTIF(N5:N28,"&gt;"&amp;N33)</f>
+      <c r="Q34" s="7">
+        <f>COUNTIF(Q5:Q28,"&gt;"&amp;Q33)</f>
         <v>0</v>
       </c>
-      <c r="O34" s="7"/>
-      <c r="P34" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q34" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R34" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="R34" s="7"/>
       <c r="S34" s="7" t="s">
         <v>26</v>
       </c>
@@ -5768,17 +5888,26 @@
       <c r="U34" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
+      <c r="V34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X34" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+      <c r="AF34" s="1"/>
+      <c r="AG34" s="1"/>
     </row>
-    <row r="35" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>28</v>
       </c>
@@ -5819,24 +5948,24 @@
       <c r="L35" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M35" s="7">
-        <f>M34/24*100</f>
+      <c r="M35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="P35" s="7">
+        <f>P34/24*100</f>
         <v>0</v>
       </c>
-      <c r="N35" s="7">
-        <f>N34/24*100</f>
+      <c r="Q35" s="7">
+        <f>Q34/24*100</f>
         <v>0</v>
       </c>
-      <c r="O35" s="7"/>
-      <c r="P35" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q35" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R35" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="R35" s="7"/>
       <c r="S35" s="7" t="s">
         <v>26</v>
       </c>
@@ -5846,17 +5975,26 @@
       <c r="U35" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-      <c r="X35" s="1"/>
+      <c r="V35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X35" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
+      <c r="AE35" s="1"/>
+      <c r="AF35" s="1"/>
+      <c r="AG35" s="1"/>
     </row>
-    <row r="36" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>29</v>
       </c>
@@ -5880,17 +6018,20 @@
       <c r="S36" s="16"/>
       <c r="T36" s="16"/>
       <c r="U36" s="16"/>
-      <c r="V36" s="1"/>
-      <c r="W36" s="1"/>
-      <c r="X36" s="1"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="16"/>
+      <c r="X36" s="16"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+      <c r="AF36" s="1"/>
+      <c r="AG36" s="1"/>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -5912,17 +6053,20 @@
       <c r="S37" s="16"/>
       <c r="T37" s="16"/>
       <c r="U37" s="16"/>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="1"/>
+      <c r="V37" s="16"/>
+      <c r="W37" s="16"/>
+      <c r="X37" s="16"/>
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
+      <c r="AF37" s="1"/>
+      <c r="AG37" s="1"/>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -5944,17 +6088,20 @@
       <c r="S38" s="16"/>
       <c r="T38" s="16"/>
       <c r="U38" s="16"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="16"/>
+      <c r="X38" s="16"/>
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
+      <c r="AG38" s="1"/>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -5976,17 +6123,20 @@
       <c r="S39" s="16"/>
       <c r="T39" s="16"/>
       <c r="U39" s="16"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-      <c r="X39" s="1"/>
+      <c r="V39" s="16"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="16"/>
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="1"/>
+      <c r="AG39" s="1"/>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -6008,24 +6158,27 @@
       <c r="S40" s="16"/>
       <c r="T40" s="16"/>
       <c r="U40" s="16"/>
-      <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
-      <c r="X40" s="1"/>
+      <c r="V40" s="16"/>
+      <c r="W40" s="16"/>
+      <c r="X40" s="16"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
+      <c r="AE40" s="1"/>
+      <c r="AF40" s="1"/>
+      <c r="AG40" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A36:A40"/>
-    <mergeCell ref="B36:U40"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="B36:X40"/>
+    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="A2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="V3:W3"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>